<commit_message>
Added Benchmark Excel spreadsheet
</commit_message>
<xml_diff>
--- a/OneToManyMapBenchmarks.xlsx
+++ b/OneToManyMapBenchmarks.xlsx
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +106,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -115,13 +129,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Segoe UI Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="0"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
@@ -171,13 +178,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -232,7 +240,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>OneToMany DataStructure Comparison</a:t>
+              <a:t>OneToManyMap DataStructure Comparison</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -828,7 +836,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-52C1-4AFE-B414-7D3EB916F210}"/>
+              <c16:uniqueId val="{00000000-939D-4FB5-8700-D5E0D5DB7E69}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1085,9 +1093,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.873816393545067E-2"/>
-          <c:y val="9.616933979602936E-2"/>
-          <c:w val="0.16463825350880029"/>
-          <c:h val="0.21923414176358771"/>
+          <c:y val="6.791615014610887E-2"/>
+          <c:w val="0.17318221901360475"/>
+          <c:h val="0.2627005873788501"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2040,237 +2048,238 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>67.34</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>151.80799999999999</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>363.24400000000003</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>608.43399999999997</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>834.23299999999995</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>1080.9749999999999</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>1375.7819999999999</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="4">
         <v>1618.6980000000001</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <v>1864.001</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="4">
         <v>2087.4470000000001</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="4">
         <v>2417.06</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>5471.6940000000004</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>8264.0730000000003</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>64.138999999999996</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>156.99</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>370.68599999999998</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>598.67999999999995</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>845.93499999999995</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>1089.9839999999999</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>1388.0889999999999</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>1649.3720000000001</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>1960.1379999999999</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>2283.7930000000001</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="4">
         <v>2513</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>5965.4539999999997</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>9027.2379999999994</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>13.522</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>50.249000000000002</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>196.95599999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>431.589</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>758.84299999999996</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>1217.81</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>1746.297</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>2509.84</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>3088.7040000000002</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>3898.3850000000002</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>4751.6120000000001</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>19033.249</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>42242.718999999997</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>2.5310000000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>5.141</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>10.417</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>17.288</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>23.821999999999999</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>27.033999999999999</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>36.183999999999997</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>39.774999999999999</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>46.171999999999997</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>52.741</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>54.65</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>111.53700000000001</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>178.114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Data Driven (Parameterized) unit tests
</commit_message>
<xml_diff>
--- a/OneToManyMapBenchmarks.xlsx
+++ b/OneToManyMapBenchmarks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c102116\Source\Repos\OneToManyMapBenchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivk\source\repos\matlus\OneToManyMapBenchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDC019B-D361-4B99-9E00-581B4EC04605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="11655"/>
+    <workbookView xWindow="420" yWindow="105" windowWidth="28005" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>OneToManyMapDataTable</t>
   </si>
@@ -76,31 +77,30 @@
   <si>
     <t>3000 -(676)</t>
   </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Gen 0</t>
+  </si>
+  <si>
+    <t>Allocated</t>
+  </si>
+  <si>
+    <t>696000 B</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,22 +113,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="0"/>
-      <name val="Segoe UI Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
@@ -142,11 +141,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,44 +154,376 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+  <cellStyles count="2">
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -372,43 +703,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>67.34</c:v>
+                  <c:v>44.628999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151.80799999999999</c:v>
+                  <c:v>100.95399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>363.24400000000003</c:v>
+                  <c:v>236.392</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>608.43399999999997</c:v>
+                  <c:v>385.50799999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>834.23299999999995</c:v>
+                  <c:v>541.29999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1080.9749999999999</c:v>
+                  <c:v>703.44299999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1375.7819999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1618.6980000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1864.001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2087.4470000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2417.06</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5471.6940000000004</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8264.0730000000003</c:v>
+                  <c:v>870.92899999999997</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0.00">
+                  <c:v>1040.826</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>1225.1679999999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0.00">
+                  <c:v>1398.6579999999999</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0.00">
+                  <c:v>1586.09</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0.00">
+                  <c:v>3486.8380000000002</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0.00">
+                  <c:v>5579.4669999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -512,43 +843,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>64.138999999999996</c:v>
+                  <c:v>39.484000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.99</c:v>
+                  <c:v>93.075000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>370.68599999999998</c:v>
+                  <c:v>220.601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>598.67999999999995</c:v>
+                  <c:v>373.30799999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>845.93499999999995</c:v>
+                  <c:v>520.83600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1089.9839999999999</c:v>
+                  <c:v>669.19100000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1388.0889999999999</c:v>
+                  <c:v>854.36500000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1649.3720000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1960.1379999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2283.7930000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2513</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5965.4539999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9027.2379999999994</c:v>
+                  <c:v>984.61099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>1139.7809999999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0.00">
+                  <c:v>1381.1010000000001</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0.00">
+                  <c:v>1479.626</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0.00">
+                  <c:v>3421.1280000000002</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0.00">
+                  <c:v>5411.0739999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,43 +983,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>13.522</c:v>
+                  <c:v>8.9459999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.249000000000002</c:v>
+                  <c:v>32.917000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>196.95599999999999</c:v>
+                  <c:v>126.54900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>431.589</c:v>
+                  <c:v>11.096</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>758.84299999999996</c:v>
+                  <c:v>488.012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1217.81</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1746.297</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2509.84</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3088.7040000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3898.3850000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4751.6120000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19033.249</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42242.718999999997</c:v>
+                  <c:v>759.29499999999996</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0.00">
+                  <c:v>1094.037</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0.00">
+                  <c:v>1479.51</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>1939.4659999999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0.00">
+                  <c:v>2452.556</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0.00">
+                  <c:v>3093.0610000000001</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0.00">
+                  <c:v>12469.946</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0.00">
+                  <c:v>28419.517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,43 +1123,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2.5310000000000001</c:v>
+                  <c:v>1.748</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.141</c:v>
+                  <c:v>3.5019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.417</c:v>
+                  <c:v>7.0359999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17.288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.821999999999999</c:v>
+                  <c:v>15.679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.033999999999999</c:v>
+                  <c:v>18.169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.183999999999997</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.774999999999999</c:v>
+                  <c:v>26.227</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46.171999999999997</c:v>
+                  <c:v>31.178000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.741</c:v>
+                  <c:v>36.146999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54.65</c:v>
+                  <c:v>36.148000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>111.53700000000001</c:v>
+                  <c:v>72.822000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>178.114</c:v>
+                  <c:v>116.331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1712,15 +2043,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1746,6 +2077,31 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B168CA99-78C5-4506-8196-29813C9DD96C}" name="Table5" displayName="Table5" ref="A1:P5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="40% - Accent5">
+  <autoFilter ref="A1:P5" xr:uid="{94FD868C-5FD6-4EE5-B092-82764261CCFD}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{172B48A2-26C4-4791-869A-4655ACBE5AE5}" name="Column1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{2E12664F-2F52-447C-B601-A29A34D7BA2F}" name="50-(10)" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{78CE9759-0F48-40F5-84E9-14E714C48996}" name="100 - (24)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{D02E4727-55C6-4E69-A908-56E5B04F6A81}" name="200 - (40)" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{5228EA0A-32FC-4A22-9B6F-1E2D019D3301}" name="300 - (69)" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{2E71520E-7F7D-4FD3-BDC0-10E9E59DC5C9}" name="400 - (84)" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{2BE28371-993D-4BB2-951A-A9333211A360}" name="500 - (108)" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{E2EA85D7-C6D1-4D65-BEA6-6752B60469A8}" name="600 - (137)" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{2E85B1FD-E6B0-45D1-9351-691F47E6F11A}" name="700 - (166)" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{5D8C34BD-5718-4A65-9CFF-8A4EA56AF0E1}" name="800 - (173)" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{AFE9C42F-AE4D-43D1-897A-3933831BABBF}" name="900 - (204)" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{437081BF-551C-44BB-B306-77B15B6C3B34}" name="1000 - (209)" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{1E7D662E-AF56-4356-A61D-C3D90D3363F2}" name="2000 - (434)" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{FB75DE4F-7134-4D3A-B6D2-7444F742FC13}" name="3000 -(676)" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{882F8BB0-3440-429D-952C-081DE4079922}" name="Gen 0" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{F1216D65-5982-4653-9A30-DB32AB2AD44A}" name="Allocated" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2044,247 +2400,307 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="O1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>67.34</v>
-      </c>
-      <c r="C2" s="4">
-        <v>151.80799999999999</v>
-      </c>
-      <c r="D2" s="4">
-        <v>363.24400000000003</v>
-      </c>
-      <c r="E2" s="4">
-        <v>608.43399999999997</v>
-      </c>
-      <c r="F2" s="4">
-        <v>834.23299999999995</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1080.9749999999999</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1375.7819999999999</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1618.6980000000001</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1864.001</v>
-      </c>
-      <c r="K2" s="4">
-        <v>2087.4470000000001</v>
-      </c>
-      <c r="L2" s="4">
-        <v>2417.06</v>
-      </c>
-      <c r="M2" s="4">
-        <v>5471.6940000000004</v>
-      </c>
-      <c r="N2" s="4">
-        <v>8264.0730000000003</v>
-      </c>
+      <c r="B2" s="2">
+        <v>44.628999999999998</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100.95399999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>236.392</v>
+      </c>
+      <c r="E2" s="2">
+        <v>385.50799999999998</v>
+      </c>
+      <c r="F2" s="2">
+        <v>541.29999999999995</v>
+      </c>
+      <c r="G2" s="2">
+        <v>703.44299999999998</v>
+      </c>
+      <c r="H2" s="2">
+        <v>870.92899999999997</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1040.826</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1225.1679999999999</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1398.6579999999999</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1586.09</v>
+      </c>
+      <c r="M2" s="5">
+        <v>3486.8380000000002</v>
+      </c>
+      <c r="N2" s="5">
+        <v>5579.4669999999996</v>
+      </c>
+      <c r="O2" s="2">
+        <v>164.0625</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>64.138999999999996</v>
-      </c>
-      <c r="C3" s="4">
-        <v>156.99</v>
-      </c>
-      <c r="D3" s="4">
-        <v>370.68599999999998</v>
-      </c>
-      <c r="E3" s="4">
-        <v>598.67999999999995</v>
-      </c>
-      <c r="F3" s="4">
-        <v>845.93499999999995</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1089.9839999999999</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1388.0889999999999</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1649.3720000000001</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1960.1379999999999</v>
-      </c>
-      <c r="K3" s="4">
-        <v>2283.7930000000001</v>
-      </c>
-      <c r="L3" s="4">
-        <v>2513</v>
-      </c>
-      <c r="M3" s="4">
-        <v>5965.4539999999997</v>
-      </c>
-      <c r="N3" s="4">
-        <v>9027.2379999999994</v>
-      </c>
+      <c r="B3" s="2">
+        <v>39.484000000000002</v>
+      </c>
+      <c r="C3" s="2">
+        <v>93.075000000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>220.601</v>
+      </c>
+      <c r="E3" s="2">
+        <v>373.30799999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>520.83600000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>669.19100000000003</v>
+      </c>
+      <c r="H3" s="2">
+        <v>854.36500000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>984.61099999999999</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1139.7809999999999</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1381.1010000000001</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1479.626</v>
+      </c>
+      <c r="M3" s="5">
+        <v>3421.1280000000002</v>
+      </c>
+      <c r="N3" s="5">
+        <v>5411.0739999999996</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>13.522</v>
-      </c>
-      <c r="C4" s="4">
-        <v>50.249000000000002</v>
-      </c>
-      <c r="D4" s="4">
-        <v>196.95599999999999</v>
-      </c>
-      <c r="E4" s="4">
-        <v>431.589</v>
-      </c>
-      <c r="F4" s="4">
-        <v>758.84299999999996</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1217.81</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1746.297</v>
-      </c>
-      <c r="I4" s="4">
-        <v>2509.84</v>
-      </c>
-      <c r="J4" s="4">
-        <v>3088.7040000000002</v>
-      </c>
-      <c r="K4" s="4">
-        <v>3898.3850000000002</v>
-      </c>
-      <c r="L4" s="4">
-        <v>4751.6120000000001</v>
-      </c>
-      <c r="M4" s="4">
-        <v>19033.249</v>
-      </c>
-      <c r="N4" s="4">
-        <v>42242.718999999997</v>
-      </c>
+      <c r="B4" s="2">
+        <v>8.9459999999999997</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32.917000000000002</v>
+      </c>
+      <c r="D4" s="2">
+        <v>126.54900000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11.096</v>
+      </c>
+      <c r="F4" s="2">
+        <v>488.012</v>
+      </c>
+      <c r="G4" s="2">
+        <v>759.29499999999996</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1094.037</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1479.51</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1939.4659999999999</v>
+      </c>
+      <c r="K4" s="5">
+        <v>2452.556</v>
+      </c>
+      <c r="L4" s="5">
+        <v>3093.0610000000001</v>
+      </c>
+      <c r="M4" s="5">
+        <v>12469.946</v>
+      </c>
+      <c r="N4" s="5">
+        <v>28419.517</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
-        <v>2.5310000000000001</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5.141</v>
-      </c>
-      <c r="D5" s="4">
-        <v>10.417</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="B5" s="2">
+        <v>1.748</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.0359999999999996</v>
+      </c>
+      <c r="E5" s="2">
         <v>17.288</v>
       </c>
-      <c r="F5" s="4">
-        <v>23.821999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>27.033999999999999</v>
-      </c>
-      <c r="H5" s="4">
-        <v>36.183999999999997</v>
-      </c>
-      <c r="I5" s="4">
-        <v>39.774999999999999</v>
-      </c>
-      <c r="J5" s="4">
-        <v>46.171999999999997</v>
-      </c>
-      <c r="K5" s="4">
-        <v>52.741</v>
-      </c>
-      <c r="L5" s="4">
-        <v>54.65</v>
-      </c>
-      <c r="M5" s="4">
-        <v>111.53700000000001</v>
-      </c>
-      <c r="N5" s="4">
-        <v>178.114</v>
-      </c>
+      <c r="F5" s="2">
+        <v>15.679</v>
+      </c>
+      <c r="G5" s="2">
+        <v>18.169</v>
+      </c>
+      <c r="H5" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>26.227</v>
+      </c>
+      <c r="J5" s="2">
+        <v>31.178000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>36.146999999999998</v>
+      </c>
+      <c r="L5" s="2">
+        <v>36.148000000000003</v>
+      </c>
+      <c r="M5" s="2">
+        <v>72.822000000000003</v>
+      </c>
+      <c r="N5" s="2">
+        <v>116.331</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>